<commit_message>
create login-able users from spreadsheet test data
</commit_message>
<xml_diff>
--- a/src/kids_art_show/kas_test/test_data_seed.xlsx
+++ b/src/kids_art_show/kas_test/test_data_seed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronbecker/MET-CS673-Group1-TermProject/src/kids_art_show/kas_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43313BDC-8C4A-0548-8E46-28931BE8464C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422996EA-094F-3140-B32A-2BD847D1D1FB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14500" xr2:uid="{FFBFE716-3F20-8142-84D9-952CBD9803FF}"/>
   </bookViews>
@@ -72,10 +72,10 @@
     <t>RndPwd1</t>
   </si>
   <si>
-    <t>adminTest1</t>
-  </si>
-  <si>
     <t>MetCs673</t>
+  </si>
+  <si>
+    <t>metCs</t>
   </si>
 </sst>
 </file>
@@ -440,7 +440,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -519,10 +519,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
         <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
seeding both users and content creators
</commit_message>
<xml_diff>
--- a/src/kids_art_show/kas_test/test_data_seed.xlsx
+++ b/src/kids_art_show/kas_test/test_data_seed.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronbecker/MET-CS673-Group1-TermProject/src/kids_art_show/kas_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422996EA-094F-3140-B32A-2BD847D1D1FB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D09B2E-2717-FD49-BF23-58EED601E9BD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14500" xr2:uid="{FFBFE716-3F20-8142-84D9-952CBD9803FF}"/>
+    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14500" activeTab="1" xr2:uid="{FFBFE716-3F20-8142-84D9-952CBD9803FF}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
+    <sheet name="creators" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>first_name</t>
   </si>
@@ -76,6 +77,45 @@
   </si>
   <si>
     <t>metCs</t>
+  </si>
+  <si>
+    <t>profile_name</t>
+  </si>
+  <si>
+    <t>parent_account</t>
+  </si>
+  <si>
+    <t>bio</t>
+  </si>
+  <si>
+    <t>Bobby</t>
+  </si>
+  <si>
+    <t>BobbyPaints</t>
+  </si>
+  <si>
+    <t>Bobby likes to paint.</t>
+  </si>
+  <si>
+    <t>nickname</t>
+  </si>
+  <si>
+    <t>HelenSculpts</t>
+  </si>
+  <si>
+    <t>Helen</t>
+  </si>
+  <si>
+    <t>Helen likes to sculpt.</t>
+  </si>
+  <si>
+    <t>JohnnyDraws</t>
+  </si>
+  <si>
+    <t>Johnny</t>
+  </si>
+  <si>
+    <t>Johnny likes to draw.</t>
   </si>
 </sst>
 </file>
@@ -439,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254344DC-690A-D94C-A20C-8B031BE2B09B}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -537,4 +577,81 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92384B3D-EEE8-4A4C-BBDF-8C1879767AE1}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
more image upload testing scratch
</commit_message>
<xml_diff>
--- a/src/kids_art_show/kas_test/test_data_seed.xlsx
+++ b/src/kids_art_show/kas_test/test_data_seed.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronbecker/MET-CS673-Group1-TermProject/src/kids_art_show/kas_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D09B2E-2717-FD49-BF23-58EED601E9BD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE1294D-A4E7-174B-92D5-13C862D3FFD4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14500" activeTab="1" xr2:uid="{FFBFE716-3F20-8142-84D9-952CBD9803FF}"/>
+    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14500" activeTab="2" xr2:uid="{FFBFE716-3F20-8142-84D9-952CBD9803FF}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
     <sheet name="creators" sheetId="2" r:id="rId2"/>
+    <sheet name="posts" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t>first_name</t>
   </si>
@@ -116,6 +117,60 @@
   </si>
   <si>
     <t>Johnny likes to draw.</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>The Boat</t>
+  </si>
+  <si>
+    <t>Look at this boat!</t>
+  </si>
+  <si>
+    <t>sailing_boat.jpg</t>
+  </si>
+  <si>
+    <t>Dolphin</t>
+  </si>
+  <si>
+    <t>Cubism or something!</t>
+  </si>
+  <si>
+    <t>dolphin.jpg</t>
+  </si>
+  <si>
+    <t>Year of the Monkey</t>
+  </si>
+  <si>
+    <t>monkey.jpg</t>
+  </si>
+  <si>
+    <t>My House</t>
+  </si>
+  <si>
+    <t>I can paint too!</t>
+  </si>
+  <si>
+    <t>house.jpg</t>
+  </si>
+  <si>
+    <t>Owls are great!</t>
+  </si>
+  <si>
+    <t>superb, even!</t>
+  </si>
+  <si>
+    <t>owl.jpg</t>
   </si>
 </sst>
 </file>
@@ -147,9 +202,18 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -159,10 +223,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92384B3D-EEE8-4A4C-BBDF-8C1879767AE1}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -654,4 +720,100 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{054F917A-0AE5-4E48-B900-D5322AEE2FEA}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
progress on privacy levels and more
</commit_message>
<xml_diff>
--- a/src/kids_art_show/kas_test/test_data_seed.xlsx
+++ b/src/kids_art_show/kas_test/test_data_seed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronbecker/MET-CS673-Group1-TermProject/src/kids_art_show/kas_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD43F0E-5B16-A24C-9EA0-95512808C873}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D52145-AE56-7949-B626-4F8D14359526}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15440" activeTab="2" xr2:uid="{FFBFE716-3F20-8142-84D9-952CBD9803FF}"/>
+    <workbookView xWindow="31520" yWindow="1360" windowWidth="25600" windowHeight="15440" activeTab="2" xr2:uid="{FFBFE716-3F20-8142-84D9-952CBD9803FF}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
   <si>
     <t>first_name</t>
   </si>
@@ -122,9 +122,6 @@
     <t>title</t>
   </si>
   <si>
-    <t>content</t>
-  </si>
-  <si>
     <t>author</t>
   </si>
   <si>
@@ -171,6 +168,24 @@
   </si>
   <si>
     <t>owl.jpg</t>
+  </si>
+  <si>
+    <t>privacy</t>
+  </si>
+  <si>
+    <t>public</t>
+  </si>
+  <si>
+    <t>private</t>
+  </si>
+  <si>
+    <t>followers</t>
+  </si>
+  <si>
+    <t>default_privacy</t>
+  </si>
+  <si>
+    <t>description</t>
   </si>
 </sst>
 </file>
@@ -546,7 +561,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G2"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -647,10 +662,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92384B3D-EEE8-4A4C-BBDF-8C1879767AE1}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -661,7 +676,7 @@
     <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
@@ -674,8 +689,11 @@
       <c r="D1" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -688,8 +706,11 @@
       <c r="D2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -702,8 +723,11 @@
       <c r="D3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -715,6 +739,9 @@
       </c>
       <c r="D4" t="s">
         <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -724,10 +751,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{054F917A-0AE5-4E48-B900-D5322AEE2FEA}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -738,85 +765,103 @@
     <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>34</v>
-      </c>
-      <c r="B2" t="s">
-        <v>35</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>37</v>
-      </c>
-      <c r="B3" t="s">
-        <v>38</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
       </c>
       <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>40</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
       </c>
       <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>42</v>
-      </c>
-      <c r="B5" t="s">
-        <v>43</v>
       </c>
       <c r="C5" t="s">
         <v>24</v>
       </c>
       <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>45</v>
-      </c>
-      <c r="B6" t="s">
-        <v>46</v>
       </c>
       <c r="C6" t="s">
         <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>46</v>
+      </c>
+      <c r="E6" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
default privacy at user level, populate form with initial
</commit_message>
<xml_diff>
--- a/src/kids_art_show/kas_test/test_data_seed.xlsx
+++ b/src/kids_art_show/kas_test/test_data_seed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronbecker/MET-CS673-Group1-TermProject/src/kids_art_show/kas_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D52145-AE56-7949-B626-4F8D14359526}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACC4E98-3AB6-8E4B-9410-87F12ECC600B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31520" yWindow="1360" windowWidth="25600" windowHeight="15440" activeTab="2" xr2:uid="{FFBFE716-3F20-8142-84D9-952CBD9803FF}"/>
+    <workbookView xWindow="51200" yWindow="460" windowWidth="25600" windowHeight="28240" activeTab="2" xr2:uid="{FFBFE716-3F20-8142-84D9-952CBD9803FF}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -558,18 +558,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254344DC-690A-D94C-A20C-8B031BE2B09B}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -591,8 +592,11 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -614,8 +618,11 @@
       <c r="G2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -637,8 +644,11 @@
       <c r="G3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>16</v>
       </c>
@@ -653,6 +663,9 @@
       </c>
       <c r="G4" t="b">
         <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -665,7 +678,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -689,9 +702,7 @@
       <c r="D1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>51</v>
-      </c>
+      <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -706,9 +717,6 @@
       <c r="D2" t="s">
         <v>22</v>
       </c>
-      <c r="E2" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -723,9 +731,6 @@
       <c r="D3" t="s">
         <v>26</v>
       </c>
-      <c r="E3" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -739,9 +744,6 @@
       </c>
       <c r="D4" t="s">
         <v>29</v>
-      </c>
-      <c r="E4" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds more test images, light refactor of database seeding script
</commit_message>
<xml_diff>
--- a/src/kids_art_show/kas_test/test_data_seed.xlsx
+++ b/src/kids_art_show/kas_test/test_data_seed.xlsx
@@ -8,26 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronbecker/MET-CS673-Group1-TermProject/src/kids_art_show/kas_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACC4E98-3AB6-8E4B-9410-87F12ECC600B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84CB8C3-4A95-B54B-8F47-D3D2780CB2D6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="460" windowWidth="25600" windowHeight="28240" activeTab="2" xr2:uid="{FFBFE716-3F20-8142-84D9-952CBD9803FF}"/>
+    <workbookView xWindow="200" yWindow="460" windowWidth="25400" windowHeight="15460" activeTab="2" xr2:uid="{FFBFE716-3F20-8142-84D9-952CBD9803FF}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
     <sheet name="creators" sheetId="2" r:id="rId2"/>
     <sheet name="posts" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="126">
   <si>
     <t>first_name</t>
   </si>
@@ -59,9 +64,6 @@
     <t>jsmith</t>
   </si>
   <si>
-    <t>LittleBobby1</t>
-  </si>
-  <si>
     <t>Jane</t>
   </si>
   <si>
@@ -71,9 +73,6 @@
     <t>jdoe</t>
   </si>
   <si>
-    <t>RndPwd1</t>
-  </si>
-  <si>
     <t>MetCs673</t>
   </si>
   <si>
@@ -179,13 +178,238 @@
     <t>private</t>
   </si>
   <si>
-    <t>followers</t>
-  </si>
-  <si>
     <t>default_privacy</t>
   </si>
   <si>
     <t>description</t>
+  </si>
+  <si>
+    <t>Such brushwork!</t>
+  </si>
+  <si>
+    <t>animal_parade.jpg</t>
+  </si>
+  <si>
+    <t>ballerina.jpg</t>
+  </si>
+  <si>
+    <t>better_parrot.jpg</t>
+  </si>
+  <si>
+    <t>bird.jpg</t>
+  </si>
+  <si>
+    <t>caterpillar.jpg</t>
+  </si>
+  <si>
+    <t>Child_scribble_age_1y10m.jpg</t>
+  </si>
+  <si>
+    <t>flower_watercolor.jpg</t>
+  </si>
+  <si>
+    <t>happy_goat.jpg</t>
+  </si>
+  <si>
+    <t>happy_sun.jpg</t>
+  </si>
+  <si>
+    <t>Luckpine.jpg</t>
+  </si>
+  <si>
+    <t>my_pony.jpg</t>
+  </si>
+  <si>
+    <t>parrot.jpeg</t>
+  </si>
+  <si>
+    <t>pastel_butterfly.jpg</t>
+  </si>
+  <si>
+    <t>pattern_fish.jpg</t>
+  </si>
+  <si>
+    <t>pic_with_kid1.jpg</t>
+  </si>
+  <si>
+    <t>pic_with_kid2.jpg</t>
+  </si>
+  <si>
+    <t>pic_with_kid3.jpg</t>
+  </si>
+  <si>
+    <t>pic_with_kid4.jpg</t>
+  </si>
+  <si>
+    <t>pic_with_kid5.jpg</t>
+  </si>
+  <si>
+    <t>pic_with_kid6.jpg</t>
+  </si>
+  <si>
+    <t>rainbow.png</t>
+  </si>
+  <si>
+    <t>smartphone.jpg</t>
+  </si>
+  <si>
+    <t>space.jpg</t>
+  </si>
+  <si>
+    <t>two_owls.jpg</t>
+  </si>
+  <si>
+    <t>Yellow-Red-Blue.jpg</t>
+  </si>
+  <si>
+    <t>LisaFrank</t>
+  </si>
+  <si>
+    <t>Lisa</t>
+  </si>
+  <si>
+    <t>Lisa Frank makes colorful school binders that most people in this class are too young to remember.</t>
+  </si>
+  <si>
+    <t>Likes</t>
+  </si>
+  <si>
+    <t>Art</t>
+  </si>
+  <si>
+    <t>Animal Parade</t>
+  </si>
+  <si>
+    <t>Ballerina</t>
+  </si>
+  <si>
+    <t>I want to be a ballerina like mommy!</t>
+  </si>
+  <si>
+    <t>I like animals</t>
+  </si>
+  <si>
+    <t>hungry for lettuce</t>
+  </si>
+  <si>
+    <t>Caterpillar</t>
+  </si>
+  <si>
+    <t>it's springtime!</t>
+  </si>
+  <si>
+    <t>Bird</t>
+  </si>
+  <si>
+    <t>Scribbles</t>
+  </si>
+  <si>
+    <t>Still learning to draw</t>
+  </si>
+  <si>
+    <t>Flowers</t>
+  </si>
+  <si>
+    <t>watercolor!</t>
+  </si>
+  <si>
+    <t>Mr. Happy Goat</t>
+  </si>
+  <si>
+    <t>Not creepy at all…</t>
+  </si>
+  <si>
+    <t>Mr. Happy Sun</t>
+  </si>
+  <si>
+    <t>Rainbow house!</t>
+  </si>
+  <si>
+    <t>Mr. Parrot</t>
+  </si>
+  <si>
+    <t>polly want a cracker?</t>
+  </si>
+  <si>
+    <t>my favorite tree!</t>
+  </si>
+  <si>
+    <t>Pine Tree</t>
+  </si>
+  <si>
+    <t>My Pony</t>
+  </si>
+  <si>
+    <t>Get me a pony!</t>
+  </si>
+  <si>
+    <t>Parrots are great</t>
+  </si>
+  <si>
+    <t>And they can talk sometimes</t>
+  </si>
+  <si>
+    <t>Practicing</t>
+  </si>
+  <si>
+    <t>For my trapper keepers</t>
+  </si>
+  <si>
+    <t>Pattern Fish</t>
+  </si>
+  <si>
+    <t>so many textures!</t>
+  </si>
+  <si>
+    <t>Bobby Scribbling</t>
+  </si>
+  <si>
+    <t>look at 'em go!</t>
+  </si>
+  <si>
+    <t>Showing off</t>
+  </si>
+  <si>
+    <t>So good!</t>
+  </si>
+  <si>
+    <t>Pro artist</t>
+  </si>
+  <si>
+    <t>mom's not home</t>
+  </si>
+  <si>
+    <t>Glue collage</t>
+  </si>
+  <si>
+    <t>Rainbow</t>
+  </si>
+  <si>
+    <t>Not double</t>
+  </si>
+  <si>
+    <t>My phone</t>
+  </si>
+  <si>
+    <t>stare at it all the time!</t>
+  </si>
+  <si>
+    <t>Kandinsky</t>
+  </si>
+  <si>
+    <t>Fits in, right?</t>
+  </si>
+  <si>
+    <t>Two owls</t>
+  </si>
+  <si>
+    <t>better than one owl</t>
+  </si>
+  <si>
+    <t>Space adventure</t>
+  </si>
+  <si>
+    <t>Pluto isn't a planet</t>
   </si>
 </sst>
 </file>
@@ -217,7 +441,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -234,16 +458,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254344DC-690A-D94C-A20C-8B031BE2B09B}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -593,7 +828,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -607,7 +842,7 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1">
         <v>7306</v>
@@ -619,21 +854,21 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1">
         <v>25933</v>
@@ -645,15 +880,15 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -665,7 +900,547 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" t="str">
+        <f>"likeSrc"&amp;(ROW()-4)</f>
+        <v>likeSrc1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1">
+        <v>32874</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" ref="C6:C24" si="0">"likeSrc"&amp;(ROW()-4)</f>
+        <v>likeSrc2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1">
+        <v>32874</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>likeSrc3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1">
+        <v>32874</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>likeSrc4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1">
+        <v>32874</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>likeSrc5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1">
+        <v>32874</v>
+      </c>
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>likeSrc6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="1">
+        <v>32874</v>
+      </c>
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>likeSrc7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1">
+        <v>32874</v>
+      </c>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>likeSrc8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="1">
+        <v>32874</v>
+      </c>
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>likeSrc9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1">
+        <v>32874</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>likeSrc10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="1">
+        <v>32874</v>
+      </c>
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" t="str">
+        <f>"likeSrc"&amp;(ROW()-4)</f>
+        <v>likeSrc11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="1">
+        <v>32874</v>
+      </c>
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>likeSrc12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1">
+        <v>32874</v>
+      </c>
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>likeSrc13</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1">
+        <v>32874</v>
+      </c>
+      <c r="F17" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>likeSrc14</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1">
+        <v>32874</v>
+      </c>
+      <c r="F18" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>likeSrc15</v>
+      </c>
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="1">
+        <v>32874</v>
+      </c>
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>likeSrc16</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="1">
+        <v>32874</v>
+      </c>
+      <c r="F20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>likeSrc17</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="1">
+        <v>32874</v>
+      </c>
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>likeSrc18</v>
+      </c>
+      <c r="D22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="1">
+        <v>32874</v>
+      </c>
+      <c r="F22" t="b">
+        <v>0</v>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>likeSrc19</v>
+      </c>
+      <c r="D23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="1">
+        <v>32874</v>
+      </c>
+      <c r="F23" t="b">
+        <v>0</v>
+      </c>
+      <c r="G23" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>likeSrc20</v>
+      </c>
+      <c r="D24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="1">
+        <v>32874</v>
+      </c>
+      <c r="F24" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -675,10 +1450,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92384B3D-EEE8-4A4C-BBDF-8C1879767AE1}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -691,59 +1466,73 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
         <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
         <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -753,120 +1542,551 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{054F917A-0AE5-4E48-B900-D5322AEE2FEA}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>48</v>
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" t="s">
-        <v>50</v>
+        <v>32</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18" t="s">
+        <v>104</v>
+      </c>
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>112</v>
+      </c>
+      <c r="B24" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>115</v>
+      </c>
+      <c r="B26" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>114</v>
+      </c>
+      <c r="B27" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>116</v>
+      </c>
+      <c r="B28" t="s">
+        <v>117</v>
+      </c>
+      <c r="C28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>118</v>
+      </c>
+      <c r="B29" t="s">
+        <v>119</v>
+      </c>
+      <c r="C29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" t="s">
+        <v>72</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>124</v>
+      </c>
+      <c r="B30" t="s">
+        <v>125</v>
+      </c>
+      <c r="C30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" t="s">
+        <v>73</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>122</v>
+      </c>
+      <c r="B31" t="s">
+        <v>123</v>
+      </c>
+      <c r="C31" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" t="s">
+        <v>74</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:E6">
+    <sortCondition ref="D2:D6"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adds ability to seed likes by adding specified number of likes from dummy user accounts
</commit_message>
<xml_diff>
--- a/src/kids_art_show/kas_test/test_data_seed.xlsx
+++ b/src/kids_art_show/kas_test/test_data_seed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronbecker/MET-CS673-Group1-TermProject/src/kids_art_show/kas_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84CB8C3-4A95-B54B-8F47-D3D2780CB2D6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6582F2-4B0D-D742-BBB6-7315A5AE502A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="460" windowWidth="25400" windowHeight="15460" activeTab="2" xr2:uid="{FFBFE716-3F20-8142-84D9-952CBD9803FF}"/>
+    <workbookView xWindow="200" yWindow="460" windowWidth="25400" windowHeight="15460" xr2:uid="{FFBFE716-3F20-8142-84D9-952CBD9803FF}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -31,8 +31,51 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Aaron Becker</author>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{27CDECFA-37D8-9D48-8ECF-F904FC50D192}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Aaron Becker:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>There are up to 20 potential likes from users defined on previous page</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="127">
   <si>
     <t>first_name</t>
   </si>
@@ -410,13 +453,16 @@
   </si>
   <si>
     <t>Pluto isn't a planet</t>
+  </si>
+  <si>
+    <t>n_likes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -431,6 +477,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -795,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254344DC-690A-D94C-A20C-8B031BE2B09B}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1541,11 +1600,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{054F917A-0AE5-4E48-B900-D5322AEE2FEA}">
-  <dimension ref="A1:E31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{054F917A-0AE5-4E48-B900-D5322AEE2FEA}">
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1556,7 +1615,7 @@
     <col min="4" max="4" width="26.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
@@ -1572,8 +1631,11 @@
       <c r="E1" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -1589,8 +1651,11 @@
       <c r="E2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -1606,8 +1671,11 @@
       <c r="E3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1623,8 +1691,11 @@
       <c r="E4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -1640,8 +1711,11 @@
       <c r="E5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1657,8 +1731,11 @@
       <c r="E6" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>81</v>
       </c>
@@ -1674,8 +1751,11 @@
       <c r="E7" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>82</v>
       </c>
@@ -1691,8 +1771,11 @@
       <c r="E8" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>97</v>
       </c>
@@ -1708,8 +1791,11 @@
       <c r="E9" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>88</v>
       </c>
@@ -1725,8 +1811,11 @@
       <c r="E10" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>86</v>
       </c>
@@ -1742,8 +1831,11 @@
       <c r="E11" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>89</v>
       </c>
@@ -1759,8 +1851,11 @@
       <c r="E12" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>91</v>
       </c>
@@ -1776,8 +1871,11 @@
       <c r="E13" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>93</v>
       </c>
@@ -1793,8 +1891,11 @@
       <c r="E14" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>95</v>
       </c>
@@ -1810,8 +1911,11 @@
       <c r="E15" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>100</v>
       </c>
@@ -1827,8 +1931,11 @@
       <c r="E16" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>101</v>
       </c>
@@ -1844,8 +1951,11 @@
       <c r="E17" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>103</v>
       </c>
@@ -1861,8 +1971,11 @@
       <c r="E18" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>105</v>
       </c>
@@ -1878,8 +1991,11 @@
       <c r="E19" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>107</v>
       </c>
@@ -1895,8 +2011,11 @@
       <c r="E20" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>120</v>
       </c>
@@ -1912,8 +2031,11 @@
       <c r="E21" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>109</v>
       </c>
@@ -1929,8 +2051,11 @@
       <c r="E22" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>111</v>
       </c>
@@ -1946,8 +2071,11 @@
       <c r="E23" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>112</v>
       </c>
@@ -1963,8 +2091,11 @@
       <c r="E24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>113</v>
       </c>
@@ -1980,8 +2111,11 @@
       <c r="E25" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>115</v>
       </c>
@@ -1997,8 +2131,11 @@
       <c r="E26" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>114</v>
       </c>
@@ -2014,8 +2151,11 @@
       <c r="E27" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>116</v>
       </c>
@@ -2031,8 +2171,11 @@
       <c r="E28" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>118</v>
       </c>
@@ -2048,8 +2191,11 @@
       <c r="E29" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>124</v>
       </c>
@@ -2065,8 +2211,11 @@
       <c r="E30" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>122</v>
       </c>
@@ -2081,6 +2230,9 @@
       </c>
       <c r="E31" s="4" t="s">
         <v>46</v>
+      </c>
+      <c r="F31">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2088,5 +2240,6 @@
     <sortCondition ref="D2:D6"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>